<commit_message>
removing unneeded instance attributes
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -45,127 +45,85 @@
     <t>mdex:dateTime</t>
   </si>
   <si>
-    <t>Sales Channel</t>
-  </si>
-  <si>
-    <t>Sales Office</t>
-  </si>
-  <si>
     <t>ORDER_NUMBER</t>
   </si>
   <si>
     <t>Order Number</t>
   </si>
   <si>
-    <t>LINE_NUMBER</t>
-  </si>
-  <si>
-    <t>Line Number</t>
-  </si>
-  <si>
-    <t>PARTY_NAME</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>ACCOUNT_NUMBER</t>
-  </si>
-  <si>
-    <t>Customer Number</t>
-  </si>
-  <si>
-    <t>ORDER_TYPE_ID</t>
-  </si>
-  <si>
-    <t>Order Type</t>
-  </si>
-  <si>
-    <t>FLOW_STATUS_CODE</t>
-  </si>
-  <si>
-    <t>Order Status</t>
-  </si>
-  <si>
-    <t>TRANSACTIONAL_CURR_CODE</t>
-  </si>
-  <si>
-    <t>Transaction Currency</t>
-  </si>
-  <si>
-    <t>SALES_CHANNEL_CODE</t>
-  </si>
-  <si>
-    <t>ATTRIBUTE1</t>
-  </si>
-  <si>
-    <t>ORDERED_ITEM</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>PRICING_QUANTITY</t>
-  </si>
-  <si>
-    <t>mdex:int</t>
-  </si>
-  <si>
-    <t>Line Quantity</t>
-  </si>
-  <si>
-    <t>UNIT_LIST_PRICE</t>
-  </si>
-  <si>
-    <t>List Price</t>
-  </si>
-  <si>
-    <t>UNIIT_SELLING_PRICE</t>
-  </si>
-  <si>
-    <t>Customer Price</t>
-  </si>
-  <si>
-    <t>USER_ITEM_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Product Description</t>
-  </si>
-  <si>
-    <t>ITEM_TYPE_CODE</t>
-  </si>
-  <si>
-    <t>Line Type</t>
-  </si>
-  <si>
-    <t>PROMISED_DATE</t>
-  </si>
-  <si>
-    <t>Promise Date</t>
-  </si>
-  <si>
     <t>SEGMENT1</t>
   </si>
   <si>
-    <t>PO Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINE_NUM </t>
-  </si>
-  <si>
-    <t>PO Line Number</t>
-  </si>
-  <si>
-    <t>UNIT_PRICE</t>
-  </si>
-  <si>
-    <t>PO Line Price</t>
-  </si>
-  <si>
-    <t>QUANTITY</t>
-  </si>
-  <si>
-    <t>PO Line Quantity</t>
+    <t>Project Number</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>ORDER_BOOK_DATE</t>
+  </si>
+  <si>
+    <t>Order Bridged Date</t>
+  </si>
+  <si>
+    <t>WWAPC</t>
+  </si>
+  <si>
+    <t>SO_CURRENCY_CODE</t>
+  </si>
+  <si>
+    <t>SO Currency</t>
+  </si>
+  <si>
+    <t>REVENUE_VALUE</t>
+  </si>
+  <si>
+    <t>Revenue Value</t>
+  </si>
+  <si>
+    <t>RELEASED_AMOUNT</t>
+  </si>
+  <si>
+    <t>Shipped Revenue</t>
+  </si>
+  <si>
+    <t>BACKLOG</t>
+  </si>
+  <si>
+    <t>Backlog</t>
+  </si>
+  <si>
+    <t>FORECAST_EQP_COST</t>
+  </si>
+  <si>
+    <t>Forecast EQP Cost</t>
+  </si>
+  <si>
+    <t>SHIPPED_FCST_EQP_COST</t>
+  </si>
+  <si>
+    <t>Shipped Fcst EQP Cost</t>
+  </si>
+  <si>
+    <t>PERIOD_NAME</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>ORG_ID</t>
+  </si>
+  <si>
+    <t>OU Name</t>
+  </si>
+  <si>
+    <t>CARRYING_OUT_ORGANIZTION_ID</t>
+  </si>
+  <si>
+    <t>Organization</t>
   </si>
 </sst>
 </file>
@@ -972,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A22:A25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +964,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1023,7 +981,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1040,10 +998,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1052,32 +1010,32 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1086,15 +1044,15 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1103,134 +1061,134 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1239,109 +1197,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement writer class and refactor excel __init__
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -39,10 +39,22 @@
     <t>mdex:string</t>
   </si>
   <si>
-    <t>PA_PERIOD_NAME</t>
-  </si>
-  <si>
-    <t>PA Period</t>
+    <t>The hold steady</t>
+  </si>
+  <si>
+    <t>Boys and girls in america</t>
+  </si>
+  <si>
+    <t>sujian stevens</t>
+  </si>
+  <si>
+    <t>oh great white city</t>
+  </si>
+  <si>
+    <t>hulk</t>
+  </si>
+  <si>
+    <t>SMASH</t>
   </si>
 </sst>
 </file>
@@ -849,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,6 +910,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove += method from insert_attrs_tl_all loop
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -42,9 +42,6 @@
     <t>The hold steady</t>
   </si>
   <si>
-    <t>Boys and girls in america</t>
-  </si>
-  <si>
     <t>sujian stevens</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>SMASH</t>
+  </si>
+  <si>
+    <t>HAWKGUY</t>
   </si>
 </sst>
 </file>
@@ -864,7 +864,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -924,7 +924,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -941,7 +941,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit to fix eql init
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="endeca_attributes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -39,22 +39,10 @@
     <t>mdex:string</t>
   </si>
   <si>
-    <t>The hold steady</t>
+    <t>organization_name</t>
   </si>
   <si>
-    <t>sujian stevens</t>
-  </si>
-  <si>
-    <t>oh great white city</t>
-  </si>
-  <si>
-    <t>hulk</t>
-  </si>
-  <si>
-    <t>SMASH</t>
-  </si>
-  <si>
-    <t>HAWKGUY</t>
+    <t>Inventory Org</t>
   </si>
 </sst>
 </file>
@@ -861,7 +849,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -870,7 +858,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" customWidth="1"/>
@@ -895,7 +883,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -907,41 +895,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved xml and record id into their own methods
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -36,13 +36,22 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>currency_conversion_rate</t>
-  </si>
-  <si>
     <t>mdex:double</t>
   </si>
   <si>
-    <t>Currency Conversion Rate</t>
+    <t>mdex:string</t>
+  </si>
+  <si>
+    <t>PO Currency</t>
+  </si>
+  <si>
+    <t>Func PO Unit Price</t>
+  </si>
+  <si>
+    <t>po_currency_code</t>
+  </si>
+  <si>
+    <t>func_item_cost</t>
   </si>
 </sst>
 </file>
@@ -849,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,16 +895,33 @@
         <v>204</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>204</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove unneeded instance attributes from sql_generator
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -39,19 +39,43 @@
     <t>mdex:double</t>
   </si>
   <si>
+    <t>DENOM_RAW_COST</t>
+  </si>
+  <si>
+    <t>Cost in USD</t>
+  </si>
+  <si>
+    <t>PA_DRAFT_INVOICE</t>
+  </si>
+  <si>
+    <t>PA Draft Invoice</t>
+  </si>
+  <si>
+    <t>INVOICE_DATE</t>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>STATUS_TRX</t>
+  </si>
+  <si>
     <t>mdex:string</t>
   </si>
   <si>
-    <t>PO Currency</t>
-  </si>
-  <si>
-    <t>Func PO Unit Price</t>
-  </si>
-  <si>
-    <t>po_currency_code</t>
-  </si>
-  <si>
-    <t>func_item_cost</t>
+    <t>AR Invoice Status</t>
+  </si>
+  <si>
+    <t>REASON_CODE</t>
+  </si>
+  <si>
+    <t>AR Exception Reason</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>JOB_NAME</t>
   </si>
 </sst>
 </file>
@@ -858,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,16 +916,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>204</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
         <v>6</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -909,19 +933,87 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>204</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix main method to clear() eql writer
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -36,46 +36,19 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>mdex:double</t>
-  </si>
-  <si>
-    <t>DENOM_RAW_COST</t>
-  </si>
-  <si>
-    <t>Cost in USD</t>
-  </si>
-  <si>
-    <t>PA_DRAFT_INVOICE</t>
-  </si>
-  <si>
-    <t>PA Draft Invoice</t>
-  </si>
-  <si>
-    <t>INVOICE_DATE</t>
-  </si>
-  <si>
-    <t>Invoice Date</t>
-  </si>
-  <si>
-    <t>STATUS_TRX</t>
-  </si>
-  <si>
     <t>mdex:string</t>
   </si>
   <si>
-    <t>AR Invoice Status</t>
+    <t>PROJ_ORGANIZATION</t>
   </si>
   <si>
-    <t>REASON_CODE</t>
+    <t>Project Org</t>
   </si>
   <si>
-    <t>AR Exception Reason</t>
+    <t>PROJECT_TYPE</t>
   </si>
   <si>
-    <t>Job</t>
-  </si>
-  <si>
-    <t>JOB_NAME</t>
+    <t>Project Type</t>
   </si>
 </sst>
 </file>
@@ -882,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +898,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -939,81 +912,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
breaking down the main() method into component parts
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="5820"/>
   </bookViews>
   <sheets>
     <sheet name="endeca_attributes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -39,16 +39,10 @@
     <t>mdex:string</t>
   </si>
   <si>
-    <t>PROJ_ORGANIZATION</t>
+    <t>VENDOR_NAME</t>
   </si>
   <si>
-    <t>Project Org</t>
-  </si>
-  <si>
-    <t>PROJECT_TYPE</t>
-  </si>
-  <si>
-    <t>Project Type</t>
+    <t>Employee/Supplier</t>
   </si>
 </sst>
 </file>
@@ -855,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,23 +898,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
xml module is now reading from the spreadsheet.
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -36,13 +36,13 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>mdex:string</t>
+    <t>mdex:double</t>
   </si>
   <si>
-    <t>VENDOR_NAME</t>
+    <t>BASE_TRANSACTION_VALUE</t>
   </si>
   <si>
-    <t>Employee/Supplier</t>
+    <t>Base Transaction Value</t>
   </si>
 </sst>
 </file>
@@ -852,7 +852,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,6 +862,8 @@
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -883,7 +885,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -892,7 +894,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
fixed xml lookup table
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -36,13 +36,94 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>mdex:double</t>
-  </si>
-  <si>
-    <t>BASE_TRANSACTION_VALUE</t>
-  </si>
-  <si>
-    <t>Base Transaction Value</t>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>mdex:string</t>
+  </si>
+  <si>
+    <t>Item Number</t>
+  </si>
+  <si>
+    <t>DEFAULT_PO_NUM</t>
+  </si>
+  <si>
+    <t>PO#</t>
+  </si>
+  <si>
+    <t>REPAIR_NUMBER</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>PROBLEM_CODE</t>
+  </si>
+  <si>
+    <t>Problem Code</t>
+  </si>
+  <si>
+    <t>MODEL_NUMBER</t>
+  </si>
+  <si>
+    <t>Model Number</t>
+  </si>
+  <si>
+    <t>PROMISE_DATE</t>
+  </si>
+  <si>
+    <t>mdex:dateTime</t>
+  </si>
+  <si>
+    <t>Parts Availability Date</t>
+  </si>
+  <si>
+    <t>PRIMARY_ROOT_CAUSE</t>
+  </si>
+  <si>
+    <t>Primary Root Cause</t>
+  </si>
+  <si>
+    <t>DIAGNOSTIC_CODE</t>
+  </si>
+  <si>
+    <t>Diagnostic Code</t>
+  </si>
+  <si>
+    <t>SERVICE_CODE</t>
+  </si>
+  <si>
+    <t>Service Code</t>
+  </si>
+  <si>
+    <t>CONTRACT_NUMBER</t>
+  </si>
+  <si>
+    <t>Contract Number</t>
+  </si>
+  <si>
+    <t>INCIDENT_NUMBER</t>
+  </si>
+  <si>
+    <t>Request Number</t>
+  </si>
+  <si>
+    <t>PARTY_NAME</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>CUSTOMER_KEY</t>
+  </si>
+  <si>
+    <t>Key Customer</t>
   </si>
 </sst>
 </file>
@@ -849,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,19 +966,240 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>204</v>
+        <v>516</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>516</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>516</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>516</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>516</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>516</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>516</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>516</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>516</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>516</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>516</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>516</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>516</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>516</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting to add default dict
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -42,6 +42,18 @@
     <t>mdex:string</t>
   </si>
   <si>
+    <t>PROBLEM_CODE</t>
+  </si>
+  <si>
+    <t>mdex:dateTime</t>
+  </si>
+  <si>
+    <t>SERVICE_CODE</t>
+  </si>
+  <si>
+    <t>PARTY_NAME</t>
+  </si>
+  <si>
     <t>Item Number</t>
   </si>
   <si>
@@ -63,9 +75,6 @@
     <t>Serial Number</t>
   </si>
   <si>
-    <t>PROBLEM_CODE</t>
-  </si>
-  <si>
     <t>Problem Code</t>
   </si>
   <si>
@@ -78,9 +87,6 @@
     <t>PROMISE_DATE</t>
   </si>
   <si>
-    <t>mdex:dateTime</t>
-  </si>
-  <si>
     <t>Parts Availability Date</t>
   </si>
   <si>
@@ -96,9 +102,6 @@
     <t>Diagnostic Code</t>
   </si>
   <si>
-    <t>SERVICE_CODE</t>
-  </si>
-  <si>
     <t>Service Code</t>
   </si>
   <si>
@@ -114,9 +117,6 @@
     <t>Request Number</t>
   </si>
   <si>
-    <t>PARTY_NAME</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
@@ -124,6 +124,24 @@
   </si>
   <si>
     <t>Key Customer</t>
+  </si>
+  <si>
+    <t>CREATION_DATE</t>
+  </si>
+  <si>
+    <t>InitDate</t>
+  </si>
+  <si>
+    <t>EVENT_DATE</t>
+  </si>
+  <si>
+    <t>AwaitP</t>
+  </si>
+  <si>
+    <t>NEED_BY_DATE</t>
+  </si>
+  <si>
+    <t>Estimated Availability Date</t>
   </si>
 </sst>
 </file>
@@ -930,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A2" sqref="A2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -986,7 +1004,7 @@
         <v>516</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -995,7 +1013,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1003,7 +1021,7 @@
         <v>516</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1012,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1020,7 +1038,7 @@
         <v>516</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1029,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1037,7 +1055,7 @@
         <v>516</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1046,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1054,7 +1072,7 @@
         <v>516</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1063,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,16 +1089,16 @@
         <v>516</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1088,7 +1106,7 @@
         <v>516</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1097,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1105,7 +1123,7 @@
         <v>516</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1114,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1122,7 +1140,7 @@
         <v>516</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1131,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1139,7 +1157,7 @@
         <v>516</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1148,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1156,7 +1174,7 @@
         <v>516</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -1165,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1173,7 +1191,7 @@
         <v>516</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -1200,6 +1218,57 @@
       </c>
       <c r="E15" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>516</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>516</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>516</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xml_generator is now expecting a list
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -36,119 +36,122 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>ITEM</t>
+    <t>mdex:double</t>
   </si>
   <si>
     <t>mdex:string</t>
   </si>
   <si>
-    <t>PROBLEM_CODE</t>
-  </si>
-  <si>
     <t>mdex:dateTime</t>
   </si>
   <si>
-    <t>SERVICE_CODE</t>
-  </si>
-  <si>
-    <t>PARTY_NAME</t>
-  </si>
-  <si>
-    <t>Item Number</t>
-  </si>
-  <si>
-    <t>DEFAULT_PO_NUM</t>
-  </si>
-  <si>
-    <t>PO#</t>
-  </si>
-  <si>
-    <t>REPAIR_NUMBER</t>
-  </si>
-  <si>
-    <t>WT</t>
-  </si>
-  <si>
-    <t>SERIAL_NUMBER</t>
-  </si>
-  <si>
-    <t>Serial Number</t>
-  </si>
-  <si>
-    <t>Problem Code</t>
-  </si>
-  <si>
-    <t>MODEL_NUMBER</t>
-  </si>
-  <si>
-    <t>Model Number</t>
-  </si>
-  <si>
-    <t>PROMISE_DATE</t>
-  </si>
-  <si>
-    <t>Parts Availability Date</t>
-  </si>
-  <si>
-    <t>PRIMARY_ROOT_CAUSE</t>
-  </si>
-  <si>
-    <t>Primary Root Cause</t>
-  </si>
-  <si>
-    <t>DIAGNOSTIC_CODE</t>
-  </si>
-  <si>
-    <t>Diagnostic Code</t>
-  </si>
-  <si>
-    <t>Service Code</t>
-  </si>
-  <si>
-    <t>CONTRACT_NUMBER</t>
-  </si>
-  <si>
-    <t>Contract Number</t>
-  </si>
-  <si>
-    <t>INCIDENT_NUMBER</t>
-  </si>
-  <si>
-    <t>Request Number</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>CUSTOMER_KEY</t>
-  </si>
-  <si>
-    <t>Key Customer</t>
-  </si>
-  <si>
-    <t>CREATION_DATE</t>
-  </si>
-  <si>
-    <t>InitDate</t>
-  </si>
-  <si>
-    <t>EVENT_DATE</t>
-  </si>
-  <si>
-    <t>AwaitP</t>
-  </si>
-  <si>
-    <t>NEED_BY_DATE</t>
-  </si>
-  <si>
-    <t>Estimated Availability Date</t>
+    <t>Tipo de Servico</t>
+  </si>
+  <si>
+    <t>No. de Modelo</t>
+  </si>
+  <si>
+    <t>Descripcio de Prob</t>
+  </si>
+  <si>
+    <t>Severidad Final</t>
+  </si>
+  <si>
+    <t>W/Ticket</t>
+  </si>
+  <si>
+    <t>Scop</t>
+  </si>
+  <si>
+    <t>Fecha de Inicio</t>
+  </si>
+  <si>
+    <t>Fecha de Facturacion</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>Direccion1</t>
+  </si>
+  <si>
+    <t>Atencion</t>
+  </si>
+  <si>
+    <t>Codigo de Problema</t>
+  </si>
+  <si>
+    <t>Codigo de Rep</t>
+  </si>
+  <si>
+    <t>Severidad Inicial</t>
+  </si>
+  <si>
+    <t>Monto en Pesos</t>
+  </si>
+  <si>
+    <t>ITEM_PERMEX</t>
+  </si>
+  <si>
+    <t>REPAIR_TYPE_NAME_PERMEX</t>
+  </si>
+  <si>
+    <t>RO_PRIORITY_MEANING_PERMEX</t>
+  </si>
+  <si>
+    <t>REPAIR_NUMBER_PERMEX</t>
+  </si>
+  <si>
+    <t>ATTRIBUTE1_PERMEX</t>
+  </si>
+  <si>
+    <t>INCIDENT_DATE_PERMEX</t>
+  </si>
+  <si>
+    <t>DATE_CLOSED_PERMEX</t>
+  </si>
+  <si>
+    <t>PARTY_NAME_PERMEX</t>
+  </si>
+  <si>
+    <t>ADDRESS1_PERMEX</t>
+  </si>
+  <si>
+    <t>ADDRESS2_PERMEX</t>
+  </si>
+  <si>
+    <t>SHIP_TO_CONTACT_PERMEX</t>
+  </si>
+  <si>
+    <t>PROBLEM_CODE_PERMEX</t>
+  </si>
+  <si>
+    <t>SERVICE_CODE_PERMEX</t>
+  </si>
+  <si>
+    <t>SEVERITY_PERMEX</t>
+  </si>
+  <si>
+    <t>EXTENDED_PRICE_PERMEX</t>
+  </si>
+  <si>
+    <t>EXTENDED_PRICE_WITH_TAX_PERMEX</t>
+  </si>
+  <si>
+    <t>PROBLEM_DESCRIPTION_PERMEX</t>
+  </si>
+  <si>
+    <t>Monto Total en Pesos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +285,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -625,8 +640,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -951,7 +968,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +1004,7 @@
         <v>516</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -996,7 +1013,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,7 +1021,7 @@
         <v>516</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1013,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,7 +1038,7 @@
         <v>516</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1030,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,7 +1055,7 @@
         <v>516</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1046,8 +1063,8 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1055,7 +1072,7 @@
         <v>516</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1064,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,7 +1089,7 @@
         <v>516</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1081,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,16 +1106,16 @@
         <v>516</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
         <v>8</v>
       </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,16 +1123,16 @@
         <v>516</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1123,7 +1140,7 @@
         <v>516</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1131,8 +1148,8 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>26</v>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,7 +1157,7 @@
         <v>516</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1148,8 +1165,8 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>27</v>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1157,7 +1174,7 @@
         <v>516</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1165,8 +1182,8 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>29</v>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,7 +1191,7 @@
         <v>516</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -1182,8 +1199,8 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
-        <v>31</v>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1191,7 +1208,7 @@
         <v>516</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -1199,8 +1216,8 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
+      <c r="E14" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,7 +1225,7 @@
         <v>516</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1216,8 +1233,8 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
-        <v>34</v>
+      <c r="E15" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,16 +1242,16 @@
         <v>516</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,16 +1259,16 @@
         <v>516</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>6</v>
       </c>
-      <c r="E17" t="s">
-        <v>38</v>
+      <c r="E17" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,13 +1279,13 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D18">
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improving user iteraction and main()
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -42,88 +42,43 @@
     <t>mdex:dateTime</t>
   </si>
   <si>
-    <t>Item Number</t>
-  </si>
-  <si>
-    <t>CREATION_DATE</t>
-  </si>
-  <si>
-    <t>REPORT_RUN_DATE</t>
-  </si>
-  <si>
-    <t>Report Run Date</t>
-  </si>
-  <si>
     <t>LINE_ID</t>
   </si>
   <si>
-    <t>Order Line ID</t>
-  </si>
-  <si>
     <t>REQUEST_DATE</t>
   </si>
   <si>
-    <t>CRSD</t>
-  </si>
-  <si>
-    <t>LINE_NUMBER</t>
-  </si>
-  <si>
-    <t>Sales Order Line</t>
-  </si>
-  <si>
-    <t>OPEN_FLAG</t>
-  </si>
-  <si>
-    <t>Line Open Flag</t>
-  </si>
-  <si>
     <t>SHIPMENT_PRIORITY_CODE</t>
   </si>
   <si>
-    <t>Shipment Priority</t>
-  </si>
-  <si>
-    <t>ORDER_NUMBER</t>
-  </si>
-  <si>
-    <t>Sales Order Number</t>
-  </si>
-  <si>
-    <t>Hold Applied Date</t>
-  </si>
-  <si>
-    <t>ORG_ID</t>
-  </si>
-  <si>
-    <t>Org Id</t>
-  </si>
-  <si>
-    <t>RELEASED_FLAG</t>
-  </si>
-  <si>
-    <t>Released Flag</t>
-  </si>
-  <si>
-    <t>CREATED_BY</t>
-  </si>
-  <si>
-    <t>Created By</t>
-  </si>
-  <si>
-    <t>SEGMENT1</t>
-  </si>
-  <si>
-    <t>HOLD_COMMENT</t>
-  </si>
-  <si>
-    <t>Hold Comments</t>
-  </si>
-  <si>
     <t>TYPE_CODE</t>
   </si>
   <si>
-    <t>Type of Hold</t>
+    <t>ORDERED_ITEM</t>
+  </si>
+  <si>
+    <t>ORDERED_QUANTITY</t>
+  </si>
+  <si>
+    <t>mdex:int</t>
+  </si>
+  <si>
+    <t>PROMISE_DATE</t>
+  </si>
+  <si>
+    <t>SCHEDULE_SHIP_DATE</t>
+  </si>
+  <si>
+    <t>SHIPPED_QUANTITY</t>
+  </si>
+  <si>
+    <t>ACTUAL_SHIPMENT_DATE</t>
+  </si>
+  <si>
+    <t>FLOW_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>SET_NAME</t>
   </si>
 </sst>
 </file>
@@ -944,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,16 +938,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,7 +952,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1008,25 +960,19 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,33 +980,28 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,16 +1009,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,16 +1023,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,41 +1037,36 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1144,16 +1074,13 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1161,16 +1088,14 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1178,43 +1103,7 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
additions to the datatype_dictionary
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -36,92 +36,35 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>mdex:string</t>
-  </si>
-  <si>
-    <t>mdex:dateTime</t>
-  </si>
-  <si>
-    <t>LINE_ID</t>
-  </si>
-  <si>
-    <t>REQUEST_DATE</t>
-  </si>
-  <si>
-    <t>SHIPMENT_PRIORITY_CODE</t>
-  </si>
-  <si>
-    <t>TYPE_CODE</t>
-  </si>
-  <si>
-    <t>ORDERED_ITEM</t>
-  </si>
-  <si>
-    <t>ORDERED_QUANTITY</t>
-  </si>
-  <si>
-    <t>mdex:int</t>
-  </si>
-  <si>
-    <t>PROMISE_DATE</t>
-  </si>
-  <si>
-    <t>SCHEDULE_SHIP_DATE</t>
-  </si>
-  <si>
-    <t>SHIPPED_QUANTITY</t>
-  </si>
-  <si>
-    <t>ACTUAL_SHIPMENT_DATE</t>
-  </si>
-  <si>
-    <t>FLOW_STATUS_CODE</t>
-  </si>
-  <si>
-    <t>SET_NAME</t>
-  </si>
-  <si>
-    <t>LINE ID</t>
-  </si>
-  <si>
-    <t>PROMISE DATE</t>
-  </si>
-  <si>
-    <t>REQUEST DATE</t>
-  </si>
-  <si>
-    <t>SHIPPED QUANTITY</t>
-  </si>
-  <si>
-    <t>PRIORITY CODE</t>
-  </si>
-  <si>
-    <t>SHIP DATE</t>
-  </si>
-  <si>
-    <t>ITEM</t>
-  </si>
-  <si>
-    <t>QUANTITY</t>
-  </si>
-  <si>
-    <t>ACTUAL SHIPMENT DATE</t>
-  </si>
-  <si>
-    <t>FLOW STATUS Code</t>
-  </si>
-  <si>
-    <t>SET</t>
-  </si>
-  <si>
-    <t>Type</t>
+    <t>mdex:double</t>
+  </si>
+  <si>
+    <t>TAX_AMT_PEMEX</t>
+  </si>
+  <si>
+    <t>IVA en Pesos</t>
+  </si>
+  <si>
+    <t>TAX_VALUE_PEMEX</t>
+  </si>
+  <si>
+    <t>IVA en DLS</t>
+  </si>
+  <si>
+    <t>TAX_AMOUNT_PEMEX</t>
+  </si>
+  <si>
+    <t>INVOICE_AMOUNT_WITH_TAX</t>
+  </si>
+  <si>
+    <t>Monto Total en DLS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,12 +198,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -610,10 +547,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -935,21 +871,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -971,210 +905,74 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14</v>
+        <v>516</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>14</v>
+        <v>516</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>14</v>
+        <v>516</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>14</v>
+        <v>516</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sql attributes now sort by  display name
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="endeca_attributes" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">endeca_attributes!$A$2:$E$37</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
   <si>
     <t>eid_instance_id</t>
   </si>
@@ -39,25 +42,229 @@
     <t>mdex:string</t>
   </si>
   <si>
-    <t>GL_DATE_333</t>
-  </si>
-  <si>
-    <t>PROJECT_NAME_333</t>
-  </si>
-  <si>
-    <t>ENTITY_333</t>
-  </si>
-  <si>
-    <t>mdex:dateTime</t>
-  </si>
-  <si>
-    <t>GL Date</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>Entity</t>
+    <t>Order #</t>
+  </si>
+  <si>
+    <t>ORDER_NUMBER</t>
+  </si>
+  <si>
+    <t>Ship To Address</t>
+  </si>
+  <si>
+    <t>Bill To Address</t>
+  </si>
+  <si>
+    <t>Bill To Contact</t>
+  </si>
+  <si>
+    <t>Pricing Date</t>
+  </si>
+  <si>
+    <t>Shipping Method</t>
+  </si>
+  <si>
+    <t>BILL_TO_CONTACT</t>
+  </si>
+  <si>
+    <t>PRICING_DATE</t>
+  </si>
+  <si>
+    <t>BILL_TO_ADDRESS</t>
+  </si>
+  <si>
+    <t>BILL_TO_CUSTOMER_NAME</t>
+  </si>
+  <si>
+    <t>SHIPPING_METHOD</t>
+  </si>
+  <si>
+    <t>SHIP_TO_ADDRESS</t>
+  </si>
+  <si>
+    <t>Shipment Priority Code</t>
+  </si>
+  <si>
+    <t>SHIPMENT_PRIORITY_CODE</t>
+  </si>
+  <si>
+    <t>Line #</t>
+  </si>
+  <si>
+    <t>Item Number</t>
+  </si>
+  <si>
+    <t>Line Quantity</t>
+  </si>
+  <si>
+    <t>Quantity Cancelled</t>
+  </si>
+  <si>
+    <t>Shipped Quantity</t>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>Unit Selling Price</t>
+  </si>
+  <si>
+    <t>Extended Price</t>
+  </si>
+  <si>
+    <t>Requested Date</t>
+  </si>
+  <si>
+    <t>Scheduled Arrival Date</t>
+  </si>
+  <si>
+    <t>Scheduled Ship Date</t>
+  </si>
+  <si>
+    <t>Promise Date</t>
+  </si>
+  <si>
+    <t>Requested Arrival Date</t>
+  </si>
+  <si>
+    <t>Ship Tracking Number</t>
+  </si>
+  <si>
+    <t>Line Status Code</t>
+  </si>
+  <si>
+    <t>Line Hold Name</t>
+  </si>
+  <si>
+    <t>Line Hold Comment</t>
+  </si>
+  <si>
+    <t>Line Type</t>
+  </si>
+  <si>
+    <t>Ship Set</t>
+  </si>
+  <si>
+    <t>Arrival Set</t>
+  </si>
+  <si>
+    <t>Fulfillment Set</t>
+  </si>
+  <si>
+    <t>Ship To Customer Name</t>
+  </si>
+  <si>
+    <t>Bill to Customer Name</t>
+  </si>
+  <si>
+    <t>Deliver To Location</t>
+  </si>
+  <si>
+    <t>Deliver to Contact</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>REFERENCE_VALUE</t>
+  </si>
+  <si>
+    <t>Service Start Date</t>
+  </si>
+  <si>
+    <t>Service End Date</t>
+  </si>
+  <si>
+    <t>Service Duration</t>
+  </si>
+  <si>
+    <t>ARRIVAL_SET_1</t>
+  </si>
+  <si>
+    <t>DELIVER_TO_LOCATION</t>
+  </si>
+  <si>
+    <t>LINE_HOLD_COMMENT</t>
+  </si>
+  <si>
+    <t>LINE_HOLD_NAME</t>
+  </si>
+  <si>
+    <t>DELIVER_TO_ADDRESS</t>
+  </si>
+  <si>
+    <t>EXTENDED_PRICE</t>
+  </si>
+  <si>
+    <t>FULFILLMENT_SET</t>
+  </si>
+  <si>
+    <t>PROMISE_DATE</t>
+  </si>
+  <si>
+    <t>ORDERED_ITEM</t>
+  </si>
+  <si>
+    <t>LINE_NUMBER</t>
+  </si>
+  <si>
+    <t>ORDERED_QUANTITY</t>
+  </si>
+  <si>
+    <t>FLOW_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>LINE_TYPE_ID</t>
+  </si>
+  <si>
+    <t>UNIT_LIST_PRICE</t>
+  </si>
+  <si>
+    <t>CANCELLED_QUANTITY</t>
+  </si>
+  <si>
+    <t>REFERENCE</t>
+  </si>
+  <si>
+    <t>FMT_REQUEST_DATE</t>
+  </si>
+  <si>
+    <t>REQUEST_DATE</t>
+  </si>
+  <si>
+    <t>Return Reason</t>
+  </si>
+  <si>
+    <t>RETURN_REASON</t>
+  </si>
+  <si>
+    <t>SERVICE_DURATION</t>
+  </si>
+  <si>
+    <t>SHIP_SET</t>
+  </si>
+  <si>
+    <t>FMT_SCHEDULE_ARRIVAL_DATE</t>
+  </si>
+  <si>
+    <t>SCHEDULE_SHIP_DATE</t>
+  </si>
+  <si>
+    <t>SERVICE_END_DATE</t>
+  </si>
+  <si>
+    <t>SERVICE_START_DATE</t>
+  </si>
+  <si>
+    <t>SHIP_TO_CUSTOMER_NAME</t>
+  </si>
+  <si>
+    <t>WAYBILL_AIRBILL_NUM</t>
+  </si>
+  <si>
+    <t>SHIPPED_QUNATITY</t>
+  </si>
+  <si>
+    <t>UNIT_SELLING_PRICE</t>
   </si>
 </sst>
 </file>
@@ -864,18 +1071,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="45.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -898,16 +1105,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -915,10 +1122,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -927,27 +1134,625 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="E2:E40">
+    <sortCondition ref="E2:E40"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
start of property test methods
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -42,10 +42,10 @@
     <t>mdex:string</t>
   </si>
   <si>
-    <t>SALES_ORDER_NUMBER</t>
+    <t>accounting_period</t>
   </si>
   <si>
-    <t>Sales Order Number</t>
+    <t>Accounting Period</t>
   </si>
 </sst>
 </file>
@@ -886,7 +886,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>516</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
fix failing test in datatype dictionary
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -39,13 +39,13 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>mdex:string</t>
+    <t>REVENUE_DISTRIBUTED_DATE</t>
   </si>
   <si>
-    <t>accounting_period</t>
+    <t>mdex:dateTime</t>
   </si>
   <si>
-    <t>Accounting Period</t>
+    <t>Revenue Distributed Date</t>
   </si>
 </sst>
 </file>
@@ -855,7 +855,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,13 +886,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>204</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1</v>

</xml_diff>

<commit_message>
sql generator refactor in process
</commit_message>
<xml_diff>
--- a/endeca_attributes.xlsx
+++ b/endeca_attributes.xlsx
@@ -39,13 +39,13 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>REVENUE_DISTRIBUTED_DATE</t>
+    <t>REVENUE_STATUS</t>
   </si>
   <si>
-    <t>mdex:dateTime</t>
+    <t>mdex:string</t>
   </si>
   <si>
-    <t>Revenue Distributed Date</t>
+    <t>Revenue Status</t>
   </si>
 </sst>
 </file>
@@ -855,7 +855,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>